<commit_message>
graph isotopes and %p
</commit_message>
<xml_diff>
--- a/data/isotopes_tidy.xlsx
+++ b/data/isotopes_tidy.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Public\Sawyer Balint\RStudio\wickford_cores\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEF602E-006F-4EAF-BE23-D56C43BD9D6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F065E040-0C52-43B0-B04D-E1DD9AC71A65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{BD75F879-5F4C-4E48-B2C3-6BF6F1C23AB2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BD75F879-5F4C-4E48-B2C3-6BF6F1C23AB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,8 +36,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="23">
   <si>
     <t>Depth (cm)</t>
   </si>
@@ -183,6 +208,25 @@
   <si>
     <t>AC2</t>
   </si>
+  <si>
+    <r>
+      <t>%P</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>total</t>
+    </r>
+  </si>
+  <si>
+    <t>N:P</t>
+  </si>
 </sst>
 </file>
 
@@ -265,6 +309,959 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Calibration"/>
+      <sheetName val="Raw Data"/>
+      <sheetName val="Results"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2">
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B2">
+            <v>0</v>
+          </cell>
+          <cell r="D2" t="e">
+            <v>#N/A</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B3">
+            <v>1</v>
+          </cell>
+          <cell r="D3">
+            <v>2.0137601448007802E-2</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B4">
+            <v>2</v>
+          </cell>
+          <cell r="D4">
+            <v>2.0686392507786838E-2</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B5">
+            <v>3</v>
+          </cell>
+          <cell r="D5">
+            <v>1.9432528452445603E-2</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B6">
+            <v>4</v>
+          </cell>
+          <cell r="D6">
+            <v>2.0980764364399503E-2</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B7">
+            <v>6</v>
+          </cell>
+          <cell r="D7">
+            <v>2.2703933016127567E-2</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B8">
+            <v>8</v>
+          </cell>
+          <cell r="D8">
+            <v>2.272652117048763E-2</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B9">
+            <v>10</v>
+          </cell>
+          <cell r="D9">
+            <v>2.3774592753728965E-2</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B10">
+            <v>12</v>
+          </cell>
+          <cell r="D10">
+            <v>2.8037270185203206E-2</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B11">
+            <v>14</v>
+          </cell>
+          <cell r="D11">
+            <v>2.5778778844237085E-2</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B12">
+            <v>16</v>
+          </cell>
+          <cell r="D12">
+            <v>2.5600060754733079E-2</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B13">
+            <v>18</v>
+          </cell>
+          <cell r="D13">
+            <v>3.0544548568847443E-2</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B14">
+            <v>20</v>
+          </cell>
+          <cell r="D14">
+            <v>2.4978105548111532E-2</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B15">
+            <v>22</v>
+          </cell>
+          <cell r="D15">
+            <v>3.4307391784964496E-2</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B16">
+            <v>24</v>
+          </cell>
+          <cell r="D16">
+            <v>2.0513096170152647E-2</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B17">
+            <v>26</v>
+          </cell>
+          <cell r="D17">
+            <v>1.924032358056621E-2</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B18">
+            <v>28</v>
+          </cell>
+          <cell r="D18">
+            <v>1.5322733234037031E-2</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B19">
+            <v>30</v>
+          </cell>
+          <cell r="D19">
+            <v>1.6242843311498837E-2</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B20">
+            <v>32</v>
+          </cell>
+          <cell r="D20">
+            <v>1.629718747849581E-2</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B21">
+            <v>34</v>
+          </cell>
+          <cell r="D21">
+            <v>1.5914548175898987E-2</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B22">
+            <v>36</v>
+          </cell>
+          <cell r="D22">
+            <v>1.5966302157179629E-2</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B23">
+            <v>38</v>
+          </cell>
+          <cell r="D23">
+            <v>1.4883965789992579E-2</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B24">
+            <v>40</v>
+          </cell>
+          <cell r="D24">
+            <v>1.3942537079511593E-2</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B25">
+            <v>42</v>
+          </cell>
+          <cell r="D25">
+            <v>7.7845032350205134E-3</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B26">
+            <v>44</v>
+          </cell>
+          <cell r="D26">
+            <v>1.4103738120257989E-2</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B27">
+            <v>46</v>
+          </cell>
+          <cell r="D27">
+            <v>1.1410467745870793E-2</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B28">
+            <v>48</v>
+          </cell>
+          <cell r="D28">
+            <v>3.3869737117053406E-3</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B29">
+            <v>50</v>
+          </cell>
+          <cell r="D29">
+            <v>-4.1899129542425605E-3</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30" t="str">
+            <v>Middle</v>
+          </cell>
+          <cell r="B30">
+            <v>52</v>
+          </cell>
+          <cell r="D30">
+            <v>9.7290698275024675E-3</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B31">
+            <v>0</v>
+          </cell>
+          <cell r="D31">
+            <v>-0.1943446033019432</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B32">
+            <v>1</v>
+          </cell>
+          <cell r="D32">
+            <v>6.3136484643477962E-3</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B33">
+            <v>2</v>
+          </cell>
+          <cell r="D33">
+            <v>1.9033273951712822E-3</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B34">
+            <v>3</v>
+          </cell>
+          <cell r="D34">
+            <v>1.8410952568212412E-2</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B35">
+            <v>4</v>
+          </cell>
+          <cell r="D35">
+            <v>2.404496675758485E-2</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B36">
+            <v>6</v>
+          </cell>
+          <cell r="D36">
+            <v>2.046072838899755E-2</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B37">
+            <v>8</v>
+          </cell>
+          <cell r="D37">
+            <v>2.575957616591466E-2</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B38">
+            <v>10</v>
+          </cell>
+          <cell r="D38">
+            <v>2.5063963866606837E-2</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B39">
+            <v>12</v>
+          </cell>
+          <cell r="D39">
+            <v>2.8815592203898052E-2</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B40">
+            <v>14</v>
+          </cell>
+          <cell r="D40">
+            <v>2.2884274560660237E-2</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B41">
+            <v>16</v>
+          </cell>
+          <cell r="D41">
+            <v>2.9422245593890433E-2</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B42">
+            <v>18</v>
+          </cell>
+          <cell r="D42">
+            <v>2.2980212469113297E-2</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B43">
+            <v>20</v>
+          </cell>
+          <cell r="D43">
+            <v>3.2610158746843337E-2</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B44">
+            <v>22</v>
+          </cell>
+          <cell r="D44">
+            <v>2.0530172469149299E-2</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B45">
+            <v>24</v>
+          </cell>
+          <cell r="D45">
+            <v>1.9409109794821876E-2</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B46">
+            <v>26</v>
+          </cell>
+          <cell r="D46">
+            <v>1.8846269147771169E-2</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B47">
+            <v>28</v>
+          </cell>
+          <cell r="D47">
+            <v>1.9294678820656903E-2</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B48">
+            <v>30</v>
+          </cell>
+          <cell r="D48">
+            <v>1.7333702980428321E-2</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B49">
+            <v>32</v>
+          </cell>
+          <cell r="D49">
+            <v>2.1330403571997846E-2</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B50">
+            <v>34</v>
+          </cell>
+          <cell r="D50">
+            <v>1.8990031425271454E-2</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B51">
+            <v>36</v>
+          </cell>
+          <cell r="D51">
+            <v>2.44081360163136E-2</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="A52" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B52">
+            <v>38</v>
+          </cell>
+          <cell r="D52">
+            <v>2.1354420674779745E-2</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="A53" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B53">
+            <v>40</v>
+          </cell>
+          <cell r="D53">
+            <v>2.7164262729447542E-2</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="A54" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B54">
+            <v>42</v>
+          </cell>
+          <cell r="D54">
+            <v>2.1348176881688757E-2</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="A55" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B55">
+            <v>44</v>
+          </cell>
+          <cell r="D55">
+            <v>1.9147908353464329E-2</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="A56" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B56">
+            <v>46</v>
+          </cell>
+          <cell r="D56">
+            <v>2.0746185529100573E-2</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="A57" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B57">
+            <v>48</v>
+          </cell>
+          <cell r="D57">
+            <v>2.2465106605004063E-2</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="A58" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B58">
+            <v>50</v>
+          </cell>
+          <cell r="D58">
+            <v>1.8941678529067859E-2</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="A59" t="str">
+            <v>North</v>
+          </cell>
+          <cell r="B59">
+            <v>52</v>
+          </cell>
+          <cell r="D59">
+            <v>2.144752602170983E-2</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="A60" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B60">
+            <v>0</v>
+          </cell>
+          <cell r="D60">
+            <v>2.8602024088597428E-2</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="A61" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B61">
+            <v>1</v>
+          </cell>
+          <cell r="D61">
+            <v>2.3813352175428064E-2</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="A62" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B62">
+            <v>2</v>
+          </cell>
+          <cell r="D62">
+            <v>6.5051465009750384E-2</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="A63" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B63">
+            <v>3</v>
+          </cell>
+          <cell r="D63">
+            <v>2.15692762904406E-2</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="A64" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B64">
+            <v>4</v>
+          </cell>
+          <cell r="D64">
+            <v>2.7032579539990002E-2</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="A65" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B65">
+            <v>6</v>
+          </cell>
+          <cell r="D65">
+            <v>2.2792422849733603E-2</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="A66" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B66">
+            <v>8</v>
+          </cell>
+          <cell r="D66">
+            <v>2.9226881269340498E-2</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="A67" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B67">
+            <v>10</v>
+          </cell>
+          <cell r="D67">
+            <v>2.2079765478681752E-2</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="A68" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B68">
+            <v>12</v>
+          </cell>
+          <cell r="D68">
+            <v>2.7780075362988339E-2</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="A69" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B69">
+            <v>14</v>
+          </cell>
+          <cell r="D69">
+            <v>2.2587030359799407E-2</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="A70" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B70">
+            <v>16</v>
+          </cell>
+          <cell r="D70">
+            <v>2.6162719462449413E-2</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="A71" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B71">
+            <v>18</v>
+          </cell>
+          <cell r="D71">
+            <v>3.9756350621990622E-2</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="A72" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B72">
+            <v>20</v>
+          </cell>
+          <cell r="D72">
+            <v>2.9093449704470736E-2</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="A73" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B73">
+            <v>22</v>
+          </cell>
+          <cell r="D73">
+            <v>1.9324350539273387E-2</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="A74" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B74">
+            <v>24</v>
+          </cell>
+          <cell r="D74">
+            <v>3.1235760717642717E-2</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="A75" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B75">
+            <v>26</v>
+          </cell>
+          <cell r="D75">
+            <v>1.8403922674197902E-2</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="A76" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B76">
+            <v>28</v>
+          </cell>
+          <cell r="D76">
+            <v>3.0173507720382509E-2</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="A77" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B77">
+            <v>30</v>
+          </cell>
+          <cell r="D77">
+            <v>1.8067241296644374E-2</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="A78" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B78">
+            <v>32</v>
+          </cell>
+          <cell r="D78">
+            <v>2.7252375492557573E-2</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="A79" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B79">
+            <v>34</v>
+          </cell>
+          <cell r="D79">
+            <v>1.4942905770415326E-2</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="A80" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B80">
+            <v>36</v>
+          </cell>
+          <cell r="D80">
+            <v>2.3476392137122021E-2</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="A81" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B81">
+            <v>38</v>
+          </cell>
+          <cell r="D81">
+            <v>1.3133627928869789E-2</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="A82" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B82">
+            <v>40</v>
+          </cell>
+          <cell r="D82">
+            <v>4.0876386745793197E-3</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="A83" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B83">
+            <v>40</v>
+          </cell>
+          <cell r="D83">
+            <v>4.0876386745793197E-3</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="A84" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B84">
+            <v>42</v>
+          </cell>
+          <cell r="D84">
+            <v>-1.0204616492646387E-2</v>
+          </cell>
+        </row>
+        <row r="85">
+          <cell r="A85" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B85">
+            <v>44</v>
+          </cell>
+          <cell r="D85">
+            <v>-8.2213940082785843E-3</v>
+          </cell>
+        </row>
+        <row r="86">
+          <cell r="A86" t="str">
+            <v>South</v>
+          </cell>
+          <cell r="B86">
+            <v>46</v>
+          </cell>
+          <cell r="D86">
+            <v>-1.3813738844312076E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -564,10 +1561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2CA535F-3CE4-4E3A-A760-A276A9904565}">
-  <dimension ref="A1:O85"/>
+  <dimension ref="A1:Q85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="G74" workbookViewId="0">
+      <selection activeCell="Q80" sqref="Q80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -587,9 +1584,10 @@
     <col min="13" max="13" width="8.54296875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -635,8 +1633,14 @@
       <c r="O1" s="11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -680,8 +1684,11 @@
       <c r="O2" s="5">
         <v>9.7814009568444007</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -727,8 +1734,12 @@
       <c r="O3" s="5">
         <v>9.8515772804343094</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P3" cm="1">
+        <f t="array" ref="P3">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B3=[1]Results!$A$2:$A$86)*(C3=[1]Results!$B$2:$B$86),0))</f>
+        <v>6.3136484643477962E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -756,8 +1767,12 @@
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P4" cm="1">
+        <f t="array" ref="P4">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B4=[1]Results!$A$2:$A$86)*(C4=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.9033273951712822E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -785,8 +1800,12 @@
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P5" cm="1">
+        <f t="array" ref="P5">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B5=[1]Results!$A$2:$A$86)*(C5=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.8410952568212412E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -832,8 +1851,16 @@
       <c r="O6" s="5">
         <v>11.354361378879654</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P6" cm="1">
+        <f t="array" ref="P6">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B6=[1]Results!$A$2:$A$86)*(C6=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.404496675758485E-2</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" ref="Q3:Q66" si="0">H6/P6</f>
+        <v>17.60099247134357</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -861,8 +1888,12 @@
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P7" cm="1">
+        <f t="array" ref="P7">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B7=[1]Results!$A$2:$A$86)*(C7=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.046072838899755E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -908,8 +1939,16 @@
       <c r="O8" s="5">
         <v>11.907335356315807</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P8" cm="1">
+        <f t="array" ref="P8">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B8=[1]Results!$A$2:$A$86)*(C8=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.575957616591466E-2</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>15.084889472323642</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -937,8 +1976,12 @@
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P9" cm="1">
+        <f t="array" ref="P9">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B9=[1]Results!$A$2:$A$86)*(C9=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.5063963866606837E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -984,8 +2027,16 @@
       <c r="O10" s="5">
         <v>12.136449678390306</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P10" cm="1">
+        <f t="array" ref="P10">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B10=[1]Results!$A$2:$A$86)*(C10=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.8815592203898052E-2</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>11.351958057062598</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1013,8 +2064,12 @@
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P11" cm="1">
+        <f t="array" ref="P11">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B11=[1]Results!$A$2:$A$86)*(C11=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.2884274560660237E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1060,8 +2115,16 @@
       <c r="O12" s="5">
         <v>12.551114843461095</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P12" cm="1">
+        <f t="array" ref="P12">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B12=[1]Results!$A$2:$A$86)*(C12=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.9422245593890433E-2</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>9.4534276270915694</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1089,8 +2152,12 @@
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P13" cm="1">
+        <f t="array" ref="P13">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B13=[1]Results!$A$2:$A$86)*(C13=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.2980212469113297E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1136,8 +2203,16 @@
       <c r="O14" s="5">
         <v>11.539107570688431</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P14" cm="1">
+        <f t="array" ref="P14">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B14=[1]Results!$A$2:$A$86)*(C14=[1]Results!$B$2:$B$86),0))</f>
+        <v>3.2610158746843337E-2</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="0"/>
+        <v>7.3322070238011339</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1165,8 +2240,12 @@
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P15" cm="1">
+        <f t="array" ref="P15">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B15=[1]Results!$A$2:$A$86)*(C15=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.0530172469149299E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1212,8 +2291,16 @@
       <c r="O16" s="5">
         <v>11.446408330821752</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P16" cm="1">
+        <f t="array" ref="P16">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B16=[1]Results!$A$2:$A$86)*(C16=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.9409109794821876E-2</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="0"/>
+        <v>12.059829286455633</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1241,8 +2328,12 @@
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P17" cm="1">
+        <f t="array" ref="P17">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B17=[1]Results!$A$2:$A$86)*(C17=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.8846269147771169E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1288,8 +2379,16 @@
       <c r="O18" s="5">
         <v>11.9663429917104</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P18" cm="1">
+        <f t="array" ref="P18">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B18=[1]Results!$A$2:$A$86)*(C18=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.9294678820656903E-2</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="0"/>
+        <v>12.076510235105129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1317,8 +2416,12 @@
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P19" cm="1">
+        <f t="array" ref="P19">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B19=[1]Results!$A$2:$A$86)*(C19=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.7333702980428321E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1364,8 +2467,16 @@
       <c r="O20" s="5">
         <v>12.562573604809286</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P20" cm="1">
+        <f t="array" ref="P20">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B20=[1]Results!$A$2:$A$86)*(C20=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.1330403571997846E-2</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="0"/>
+        <v>11.946986210935949</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1393,8 +2504,12 @@
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P21" cm="1">
+        <f t="array" ref="P21">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B21=[1]Results!$A$2:$A$86)*(C21=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.8990031425271454E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1440,8 +2555,16 @@
       <c r="O22" s="5">
         <v>12.804492259695888</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P22" cm="1">
+        <f t="array" ref="P22">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B22=[1]Results!$A$2:$A$86)*(C22=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.44081360163136E-2</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="0"/>
+        <v>11.051599519697833</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1469,8 +2592,12 @@
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P23" cm="1">
+        <f t="array" ref="P23">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B23=[1]Results!$A$2:$A$86)*(C23=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.1354420674779745E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -1516,8 +2643,16 @@
       <c r="O24" s="5">
         <v>14.293519010866833</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P24" cm="1">
+        <f t="array" ref="P24">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B24=[1]Results!$A$2:$A$86)*(C24=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.7164262729447542E-2</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="0"/>
+        <v>10.624642613159924</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1545,8 +2680,12 @@
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P25" cm="1">
+        <f t="array" ref="P25">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B25=[1]Results!$A$2:$A$86)*(C25=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.1348176881688757E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -1592,8 +2731,16 @@
       <c r="O26" s="5">
         <v>14.159481527298476</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P26" cm="1">
+        <f t="array" ref="P26">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B26=[1]Results!$A$2:$A$86)*(C26=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.9147908353464329E-2</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="0"/>
+        <v>16.574586826296702</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -1621,8 +2768,12 @@
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P27" cm="1">
+        <f t="array" ref="P27">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B27=[1]Results!$A$2:$A$86)*(C27=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.0746185529100573E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -1668,8 +2819,16 @@
       <c r="O28" s="5">
         <v>13.851831077633147</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P28" cm="1">
+        <f t="array" ref="P28">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B28=[1]Results!$A$2:$A$86)*(C28=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.2465106605004063E-2</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="0"/>
+        <v>12.209499065915344</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -1697,8 +2856,12 @@
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P29" cm="1">
+        <f t="array" ref="P29">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B29=[1]Results!$A$2:$A$86)*(C29=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.8941678529067859E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -1742,8 +2905,16 @@
       <c r="O30" s="5">
         <v>14.606457108262555</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P30" cm="1">
+        <f t="array" ref="P30">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B30=[1]Results!$A$2:$A$86)*(C30=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.144752602170983E-2</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="0"/>
+        <v>12.636383861004052</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -1787,8 +2958,12 @@
       <c r="O31" s="5">
         <v>11.181973212932103</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P31" t="e" cm="1">
+        <f t="array" ref="P31">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B31=[1]Results!$A$2:$A$86)*(C31=[1]Results!$B$2:$B$86),0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -1834,8 +3009,16 @@
       <c r="O32" s="5">
         <v>10.16396977347523</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P32" cm="1">
+        <f t="array" ref="P32">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B32=[1]Results!$A$2:$A$86)*(C32=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.0137601448007802E-2</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="0"/>
+        <v>28.593922273139302</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -1863,8 +3046,12 @@
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P33" cm="1">
+        <f t="array" ref="P33">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B33=[1]Results!$A$2:$A$86)*(C33=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.0686392507786838E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1892,8 +3079,12 @@
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P34" cm="1">
+        <f t="array" ref="P34">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B34=[1]Results!$A$2:$A$86)*(C34=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.9432528452445603E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -1939,8 +3130,16 @@
       <c r="O35" s="5">
         <v>10.581245931839771</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P35" cm="1">
+        <f t="array" ref="P35">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B35=[1]Results!$A$2:$A$86)*(C35=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.0980764364399503E-2</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="0"/>
+        <v>22.902788235266978</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -1968,8 +3167,12 @@
       <c r="M36" s="5"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P36" cm="1">
+        <f t="array" ref="P36">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B36=[1]Results!$A$2:$A$86)*(C36=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.2703933016127567E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -2015,8 +3218,16 @@
       <c r="O37" s="5">
         <v>10.699198744180357</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P37" cm="1">
+        <f t="array" ref="P37">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B37=[1]Results!$A$2:$A$86)*(C37=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.272652117048763E-2</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="0"/>
+        <v>20.624393133412468</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -2044,8 +3255,12 @@
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P38" cm="1">
+        <f t="array" ref="P38">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B38=[1]Results!$A$2:$A$86)*(C38=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.3774592753728965E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -2091,8 +3306,16 @@
       <c r="O39" s="5">
         <v>11.204330598559185</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P39" cm="1">
+        <f t="array" ref="P39">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B39=[1]Results!$A$2:$A$86)*(C39=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.8037270185203206E-2</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="0"/>
+        <v>14.817292879558966</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -2120,8 +3343,12 @@
       <c r="M40" s="5"/>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P40" cm="1">
+        <f t="array" ref="P40">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B40=[1]Results!$A$2:$A$86)*(C40=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.5778778844237085E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -2167,8 +3394,16 @@
       <c r="O41" s="5">
         <v>12.292362205561304</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P41" cm="1">
+        <f t="array" ref="P41">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B41=[1]Results!$A$2:$A$86)*(C41=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.5600060754733079E-2</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="0"/>
+        <v>14.696087446506874</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -2196,8 +3431,12 @@
       <c r="M42" s="5"/>
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P42" cm="1">
+        <f t="array" ref="P42">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B42=[1]Results!$A$2:$A$86)*(C42=[1]Results!$B$2:$B$86),0))</f>
+        <v>3.0544548568847443E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -2243,8 +3482,16 @@
       <c r="O43" s="5">
         <v>14.267185193902373</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P43" cm="1">
+        <f t="array" ref="P43">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B43=[1]Results!$A$2:$A$86)*(C43=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.4978105548111532E-2</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="0"/>
+        <v>11.618950047156146</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -2272,8 +3519,12 @@
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
       <c r="O44" s="5"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P44" cm="1">
+        <f t="array" ref="P44">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B44=[1]Results!$A$2:$A$86)*(C44=[1]Results!$B$2:$B$86),0))</f>
+        <v>3.4307391784964496E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -2319,8 +3570,16 @@
       <c r="O45" s="5">
         <v>12.454058655356684</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P45" cm="1">
+        <f t="array" ref="P45">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B45=[1]Results!$A$2:$A$86)*(C45=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.0513096170152647E-2</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="0"/>
+        <v>11.287219466974859</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -2348,8 +3607,12 @@
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P46" cm="1">
+        <f t="array" ref="P46">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B46=[1]Results!$A$2:$A$86)*(C46=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.924032358056621E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -2395,8 +3658,16 @@
       <c r="O47" s="5">
         <v>12.884726728882482</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P47" cm="1">
+        <f t="array" ref="P47">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B47=[1]Results!$A$2:$A$86)*(C47=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.5322733234037031E-2</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="0"/>
+        <v>15.667680303073313</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -2424,8 +3695,12 @@
       <c r="M48" s="5"/>
       <c r="N48" s="5"/>
       <c r="O48" s="5"/>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P48" cm="1">
+        <f t="array" ref="P48">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B48=[1]Results!$A$2:$A$86)*(C48=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.6242843311498837E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -2471,8 +3746,16 @@
       <c r="O49" s="5">
         <v>12.347016684948125</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P49" cm="1">
+        <f t="array" ref="P49">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B49=[1]Results!$A$2:$A$86)*(C49=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.629718747849581E-2</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="0"/>
+        <v>13.407869783483452</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -2500,8 +3783,12 @@
       <c r="M50" s="5"/>
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P50" cm="1">
+        <f t="array" ref="P50">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B50=[1]Results!$A$2:$A$86)*(C50=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.5914548175898987E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>12</v>
       </c>
@@ -2547,8 +3834,16 @@
       <c r="O51" s="5">
         <v>11.353948422178279</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P51" cm="1">
+        <f t="array" ref="P51">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B51=[1]Results!$A$2:$A$86)*(C51=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.5966302157179629E-2</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" si="0"/>
+        <v>14.311130598934628</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -2576,8 +3871,12 @@
       <c r="M52" s="5"/>
       <c r="N52" s="5"/>
       <c r="O52" s="5"/>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P52" cm="1">
+        <f t="array" ref="P52">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B52=[1]Results!$A$2:$A$86)*(C52=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.4883965789992579E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -2623,8 +3922,16 @@
       <c r="O53" s="5">
         <v>11.230043612671645</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P53" cm="1">
+        <f t="array" ref="P53">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B53=[1]Results!$A$2:$A$86)*(C53=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.3942537079511593E-2</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="0"/>
+        <v>14.644604269957249</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -2652,8 +3959,12 @@
       <c r="M54" s="5"/>
       <c r="N54" s="5"/>
       <c r="O54" s="5"/>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P54" cm="1">
+        <f t="array" ref="P54">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B54=[1]Results!$A$2:$A$86)*(C54=[1]Results!$B$2:$B$86),0))</f>
+        <v>7.7845032350205134E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -2699,8 +4010,16 @@
       <c r="O55" s="5">
         <v>11.51071938939462</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P55" cm="1">
+        <f t="array" ref="P55">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B55=[1]Results!$A$2:$A$86)*(C55=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.4103738120257989E-2</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" si="0"/>
+        <v>15.403451380447644</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -2728,8 +4047,12 @@
       <c r="M56" s="5"/>
       <c r="N56" s="5"/>
       <c r="O56" s="5"/>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P56" cm="1">
+        <f t="array" ref="P56">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B56=[1]Results!$A$2:$A$86)*(C56=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.1410467745870793E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>12</v>
       </c>
@@ -2775,8 +4098,16 @@
       <c r="O57" s="5">
         <v>15.181986460882234</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P57" cm="1">
+        <f t="array" ref="P57">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B57=[1]Results!$A$2:$A$86)*(C57=[1]Results!$B$2:$B$86),0))</f>
+        <v>3.3869737117053406E-3</v>
+      </c>
+      <c r="Q57">
+        <f t="shared" si="0"/>
+        <v>38.222827272706198</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>12</v>
       </c>
@@ -2804,8 +4135,12 @@
       <c r="M58" s="5"/>
       <c r="N58" s="5"/>
       <c r="O58" s="5"/>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P58" cm="1">
+        <f t="array" ref="P58">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B58=[1]Results!$A$2:$A$86)*(C58=[1]Results!$B$2:$B$86),0))</f>
+        <v>-4.1899129542425605E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>12</v>
       </c>
@@ -2849,8 +4184,16 @@
       <c r="O59" s="5">
         <v>20.527435225542579</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P59" cm="1">
+        <f t="array" ref="P59">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B59=[1]Results!$A$2:$A$86)*(C59=[1]Results!$B$2:$B$86),0))</f>
+        <v>9.7290698275024675E-3</v>
+      </c>
+      <c r="Q59">
+        <f t="shared" si="0"/>
+        <v>12.816809411257482</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>13</v>
       </c>
@@ -2894,8 +4237,16 @@
       <c r="O60" s="5">
         <v>12.264433507010711</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P60" cm="1">
+        <f t="array" ref="P60">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B60=[1]Results!$A$2:$A$86)*(C60=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.8602024088597428E-2</v>
+      </c>
+      <c r="Q60">
+        <f t="shared" si="0"/>
+        <v>20.398942752852946</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>13</v>
       </c>
@@ -2941,8 +4292,16 @@
       <c r="O61" s="5">
         <v>11.513460440941229</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P61" cm="1">
+        <f t="array" ref="P61">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B61=[1]Results!$A$2:$A$86)*(C61=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.3813352175428064E-2</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="0"/>
+        <v>17.590427377462458</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>13</v>
       </c>
@@ -2970,8 +4329,12 @@
       <c r="M62" s="5"/>
       <c r="N62" s="5"/>
       <c r="O62" s="5"/>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P62" cm="1">
+        <f t="array" ref="P62">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B62=[1]Results!$A$2:$A$86)*(C62=[1]Results!$B$2:$B$86),0))</f>
+        <v>6.5051465009750384E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>13</v>
       </c>
@@ -2999,8 +4362,12 @@
       <c r="M63" s="5"/>
       <c r="N63" s="5"/>
       <c r="O63" s="5"/>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P63" cm="1">
+        <f t="array" ref="P63">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B63=[1]Results!$A$2:$A$86)*(C63=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.15692762904406E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>13</v>
       </c>
@@ -3046,8 +4413,16 @@
       <c r="O64" s="5">
         <v>11.547904250649413</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P64" cm="1">
+        <f t="array" ref="P64">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B64=[1]Results!$A$2:$A$86)*(C64=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.7032579539990002E-2</v>
+      </c>
+      <c r="Q64">
+        <f t="shared" si="0"/>
+        <v>13.520023297008377</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>13</v>
       </c>
@@ -3075,8 +4450,12 @@
       <c r="M65" s="5"/>
       <c r="N65" s="5"/>
       <c r="O65" s="5"/>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P65" cm="1">
+        <f t="array" ref="P65">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B65=[1]Results!$A$2:$A$86)*(C65=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.2792422849733603E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>13</v>
       </c>
@@ -3122,8 +4501,16 @@
       <c r="O66" s="5">
         <v>11.625079032153144</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P66" cm="1">
+        <f t="array" ref="P66">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B66=[1]Results!$A$2:$A$86)*(C66=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.9226881269340498E-2</v>
+      </c>
+      <c r="Q66">
+        <f t="shared" si="0"/>
+        <v>11.693121116825061</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>13</v>
       </c>
@@ -3151,8 +4538,12 @@
       <c r="M67" s="5"/>
       <c r="N67" s="5"/>
       <c r="O67" s="5"/>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P67" cm="1">
+        <f t="array" ref="P67">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B67=[1]Results!$A$2:$A$86)*(C67=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.2079765478681752E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>13</v>
       </c>
@@ -3198,8 +4589,16 @@
       <c r="O68" s="5">
         <v>11.98280363738818</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P68" cm="1">
+        <f t="array" ref="P68">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B68=[1]Results!$A$2:$A$86)*(C68=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.7780075362988339E-2</v>
+      </c>
+      <c r="Q68">
+        <f t="shared" ref="Q67:Q85" si="1">H68/P68</f>
+        <v>9.4270801429070819</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>13</v>
       </c>
@@ -3227,8 +4626,12 @@
       <c r="M69" s="5"/>
       <c r="N69" s="5"/>
       <c r="O69" s="5"/>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P69" cm="1">
+        <f t="array" ref="P69">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B69=[1]Results!$A$2:$A$86)*(C69=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.2587030359799407E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>13</v>
       </c>
@@ -3274,8 +4677,16 @@
       <c r="O70" s="5">
         <v>11.315851297217778</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P70" cm="1">
+        <f t="array" ref="P70">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B70=[1]Results!$A$2:$A$86)*(C70=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.6162719462449413E-2</v>
+      </c>
+      <c r="Q70">
+        <f t="shared" si="1"/>
+        <v>9.5304904401168038</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>13</v>
       </c>
@@ -3303,8 +4714,12 @@
       <c r="M71" s="5"/>
       <c r="N71" s="5"/>
       <c r="O71" s="5"/>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P71" cm="1">
+        <f t="array" ref="P71">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B71=[1]Results!$A$2:$A$86)*(C71=[1]Results!$B$2:$B$86),0))</f>
+        <v>3.9756350621990622E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>13</v>
       </c>
@@ -3350,8 +4765,16 @@
       <c r="O72" s="5">
         <v>12.178331189052706</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P72" cm="1">
+        <f t="array" ref="P72">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B72=[1]Results!$A$2:$A$86)*(C72=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.9093449704470736E-2</v>
+      </c>
+      <c r="Q72">
+        <f t="shared" si="1"/>
+        <v>8.8988303233252335</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>13</v>
       </c>
@@ -3379,8 +4802,12 @@
       <c r="M73" s="5"/>
       <c r="N73" s="5"/>
       <c r="O73" s="5"/>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P73" cm="1">
+        <f t="array" ref="P73">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B73=[1]Results!$A$2:$A$86)*(C73=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.9324350539273387E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>13</v>
       </c>
@@ -3426,8 +4853,16 @@
       <c r="O74" s="5">
         <v>12.301841667750482</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P74" cm="1">
+        <f t="array" ref="P74">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B74=[1]Results!$A$2:$A$86)*(C74=[1]Results!$B$2:$B$86),0))</f>
+        <v>3.1235760717642717E-2</v>
+      </c>
+      <c r="Q74">
+        <f t="shared" si="1"/>
+        <v>7.9579832004805002</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>13</v>
       </c>
@@ -3455,8 +4890,12 @@
       <c r="M75" s="5"/>
       <c r="N75" s="5"/>
       <c r="O75" s="5"/>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P75" cm="1">
+        <f t="array" ref="P75">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B75=[1]Results!$A$2:$A$86)*(C75=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.8403922674197902E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>13</v>
       </c>
@@ -3502,8 +4941,16 @@
       <c r="O76" s="5">
         <v>13.906547028972533</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P76" cm="1">
+        <f t="array" ref="P76">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B76=[1]Results!$A$2:$A$86)*(C76=[1]Results!$B$2:$B$86),0))</f>
+        <v>3.0173507720382509E-2</v>
+      </c>
+      <c r="Q76">
+        <f t="shared" si="1"/>
+        <v>8.193717584085098</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>13</v>
       </c>
@@ -3531,8 +4978,12 @@
       <c r="M77" s="5"/>
       <c r="N77" s="5"/>
       <c r="O77" s="5"/>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P77" cm="1">
+        <f t="array" ref="P77">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B77=[1]Results!$A$2:$A$86)*(C77=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.8067241296644374E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>13</v>
       </c>
@@ -3578,8 +5029,16 @@
       <c r="O78" s="5">
         <v>15.277239021073939</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P78" cm="1">
+        <f t="array" ref="P78">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B78=[1]Results!$A$2:$A$86)*(C78=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.7252375492557573E-2</v>
+      </c>
+      <c r="Q78">
+        <f t="shared" si="1"/>
+        <v>11.178253908437906</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>13</v>
       </c>
@@ -3607,8 +5066,12 @@
       <c r="M79" s="5"/>
       <c r="N79" s="5"/>
       <c r="O79" s="5"/>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P79" cm="1">
+        <f t="array" ref="P79">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B79=[1]Results!$A$2:$A$86)*(C79=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.4942905770415326E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>13</v>
       </c>
@@ -3654,8 +5117,16 @@
       <c r="O80" s="5">
         <v>17.301755567596683</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P80" cm="1">
+        <f t="array" ref="P80">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B80=[1]Results!$A$2:$A$86)*(C80=[1]Results!$B$2:$B$86),0))</f>
+        <v>2.3476392137122021E-2</v>
+      </c>
+      <c r="Q80">
+        <f t="shared" si="1"/>
+        <v>14.516350861888219</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>13</v>
       </c>
@@ -3683,8 +5154,12 @@
       <c r="M81" s="5"/>
       <c r="N81" s="5"/>
       <c r="O81" s="5"/>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P81" cm="1">
+        <f t="array" ref="P81">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B81=[1]Results!$A$2:$A$86)*(C81=[1]Results!$B$2:$B$86),0))</f>
+        <v>1.3133627928869789E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>13</v>
       </c>
@@ -3730,8 +5205,12 @@
       <c r="O82" s="5">
         <v>18.422287347309112</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P82" cm="1">
+        <f t="array" ref="P82">INDEX([1]Results!$D$2:$D$86,MATCH(1,(B82=[1]Results!$A$2:$A$86)*(C82=[1]Results!$B$2:$B$86),0))</f>
+        <v>4.0876386745793197E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>13</v>
       </c>
@@ -3759,8 +5238,11 @@
       <c r="M83" s="5"/>
       <c r="N83" s="5"/>
       <c r="O83" s="5"/>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>13</v>
       </c>
@@ -3806,8 +5288,11 @@
       <c r="O84" s="5">
         <v>19.66122375448662</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>13</v>
       </c>
@@ -3850,6 +5335,9 @@
       </c>
       <c r="O85" s="5">
         <v>19.435325204932532</v>
+      </c>
+      <c r="P85">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
outreach and new graphs
</commit_message>
<xml_diff>
--- a/data/isotopes_tidy.xlsx
+++ b/data/isotopes_tidy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Public\Sawyer Balint\RStudio\wickford_cores\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9934DD3C-B072-4C8D-AA2A-5D467160745B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C031B9CC-724D-4DA2-9B78-63073A5023C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BD75F879-5F4C-4E48-B2C3-6BF6F1C23AB2}"/>
   </bookViews>
@@ -1596,7 +1596,7 @@
   <dimension ref="A1:Q85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>